<commit_message>
added new scraping script for firebase connection
</commit_message>
<xml_diff>
--- a/Autostockin/ยิงรับ 49.xlsx
+++ b/Autostockin/ยิงรับ 49.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Autostockin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA781523-F4FE-495A-A830-9B1B23B4B411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC1C4A9-86CF-4FDA-B9D6-6356D42B2D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1095" windowWidth="21600" windowHeight="11295" xr2:uid="{47EFCF22-5A4D-4004-9D3D-F4E18B203E38}"/>
+    <workbookView xWindow="11025" yWindow="1425" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{47EFCF22-5A4D-4004-9D3D-F4E18B203E38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$E$250</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$E$249</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5329" uniqueCount="3927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5389" uniqueCount="3987">
   <si>
     <t xml:space="preserve">Bill Type: </t>
   </si>
@@ -11819,6 +11819,186 @@
   </si>
   <si>
     <t>+1292-1055</t>
+  </si>
+  <si>
+    <t>+1858-562</t>
+  </si>
+  <si>
+    <t>+2598-1085</t>
+  </si>
+  <si>
+    <t>+1707-944</t>
+  </si>
+  <si>
+    <t>+1070-1222</t>
+  </si>
+  <si>
+    <t>+5198-371</t>
+  </si>
+  <si>
+    <t>+4977-663</t>
+  </si>
+  <si>
+    <t>+1499-770</t>
+  </si>
+  <si>
+    <t>+407-823</t>
+  </si>
+  <si>
+    <t>+249-1520</t>
+  </si>
+  <si>
+    <t>+140-1708</t>
+  </si>
+  <si>
+    <t>+3369-743</t>
+  </si>
+  <si>
+    <t>+5545-423</t>
+  </si>
+  <si>
+    <t>+2709-724</t>
+  </si>
+  <si>
+    <t>+2754-1273</t>
+  </si>
+  <si>
+    <t>+0023-1748</t>
+  </si>
+  <si>
+    <t>+2387-795</t>
+  </si>
+  <si>
+    <t>757-1298</t>
+  </si>
+  <si>
+    <t>+1667-949</t>
+  </si>
+  <si>
+    <t>+10880-1067</t>
+  </si>
+  <si>
+    <t>+0080-1752</t>
+  </si>
+  <si>
+    <t>+7827-241</t>
+  </si>
+  <si>
+    <t>+186-1515</t>
+  </si>
+  <si>
+    <t>+743-1214</t>
+  </si>
+  <si>
+    <t>+3363-789</t>
+  </si>
+  <si>
+    <t>+1055-1305</t>
+  </si>
+  <si>
+    <t>+1225-891</t>
+  </si>
+  <si>
+    <t>+14073-64</t>
+  </si>
+  <si>
+    <t>+2849-792</t>
+  </si>
+  <si>
+    <t>+1599-840</t>
+  </si>
+  <si>
+    <t>+867-1326</t>
+  </si>
+  <si>
+    <t>+3631-856</t>
+  </si>
+  <si>
+    <t>+2003-1056</t>
+  </si>
+  <si>
+    <t>+5797-1075</t>
+  </si>
+  <si>
+    <t>+118-1503</t>
+  </si>
+  <si>
+    <t>+1081-1289</t>
+  </si>
+  <si>
+    <t>+2785-929</t>
+  </si>
+  <si>
+    <t>+9620-487</t>
+  </si>
+  <si>
+    <t>+4412-767</t>
+  </si>
+  <si>
+    <t>+2565-758</t>
+  </si>
+  <si>
+    <t>+2970-1053</t>
+  </si>
+  <si>
+    <t>+8052-671</t>
+  </si>
+  <si>
+    <t>+8651-749</t>
+  </si>
+  <si>
+    <t>+9748-619</t>
+  </si>
+  <si>
+    <t>+586-1313</t>
+  </si>
+  <si>
+    <t>+7357-650</t>
+  </si>
+  <si>
+    <t>+2803-1095</t>
+  </si>
+  <si>
+    <t>+32470-179</t>
+  </si>
+  <si>
+    <t>+629-1445</t>
+  </si>
+  <si>
+    <t>+8921-717</t>
+  </si>
+  <si>
+    <t>+0026-1762</t>
+  </si>
+  <si>
+    <t>+1060-852</t>
+  </si>
+  <si>
+    <t>+3570-446</t>
+  </si>
+  <si>
+    <t>+26536-232</t>
+  </si>
+  <si>
+    <t>+2787-798</t>
+  </si>
+  <si>
+    <t>+34912-222</t>
+  </si>
+  <si>
+    <t>+9647-458</t>
+  </si>
+  <si>
+    <t>+6240-794</t>
+  </si>
+  <si>
+    <t>+2896-484</t>
+  </si>
+  <si>
+    <t>+19013-646</t>
+  </si>
+  <si>
+    <t>+13677-240</t>
   </si>
 </sst>
 </file>
@@ -11879,7 +12059,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -12197,10 +12384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B40E757-AF6D-418F-8CB6-C916F96CFF4A}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12210,10 +12397,7 @@
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>3857</v>
-      </c>
+    <row r="1" spans="2:5">
       <c r="B1" s="1" t="s">
         <v>541</v>
       </c>
@@ -12228,392 +12412,91 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>3858</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>3859</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>3860</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>3861</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>3862</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>3863</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>3864</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>3865</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>3866</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>3867</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>3868</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>3869</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>3870</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>3871</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>3872</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
-        <v>3873</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
-        <v>3874</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>3875</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
-        <v>3876</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1" t="s">
-        <v>3877</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="1" t="s">
-        <v>3878</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="1" t="s">
-        <v>3879</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="1" t="s">
-        <v>3880</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="1" t="s">
-        <v>3881</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="1" t="s">
-        <v>3882</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="1" t="s">
-        <v>3883</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="1" t="s">
-        <v>3884</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="1" t="s">
-        <v>3885</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="1" t="s">
-        <v>3886</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="1" t="s">
-        <v>3887</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="1" t="s">
-        <v>3888</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="1" t="s">
-        <v>3889</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="1" t="s">
-        <v>3890</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
-        <v>3891</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="1" t="s">
-        <v>3892</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="1" t="s">
-        <v>3893</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="1" t="s">
-        <v>3894</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="1" t="s">
-        <v>3895</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="1" t="s">
-        <v>3896</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="1" t="s">
-        <v>3897</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="1" t="s">
-        <v>3898</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="1" t="s">
-        <v>3899</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="1" t="s">
-        <v>3900</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="1" t="s">
-        <v>3901</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="1" t="s">
-        <v>3902</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="1" t="s">
-        <v>3903</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="1" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="1" t="s">
-        <v>3905</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="1" t="s">
-        <v>3906</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="1" t="s">
-        <v>3907</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="1" t="s">
-        <v>3908</v>
-      </c>
+    <row r="51" spans="7:7">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="7:7">
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="1" t="s">
-        <v>3909</v>
-      </c>
+    <row r="53" spans="7:7">
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="1" t="s">
-        <v>3910</v>
-      </c>
+    <row r="54" spans="7:7">
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="1" t="s">
-        <v>3911</v>
-      </c>
+    <row r="55" spans="7:7">
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="1" t="s">
-        <v>3912</v>
-      </c>
+    <row r="56" spans="7:7">
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="1" t="s">
-        <v>3913</v>
-      </c>
+    <row r="57" spans="7:7">
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="1" t="s">
-        <v>3914</v>
-      </c>
+    <row r="58" spans="7:7">
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="1" t="s">
-        <v>3915</v>
-      </c>
+    <row r="59" spans="7:7">
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="1" t="s">
-        <v>3916</v>
-      </c>
+    <row r="60" spans="7:7">
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="1" t="s">
-        <v>3917</v>
-      </c>
+    <row r="61" spans="7:7">
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="1" t="s">
-        <v>3918</v>
-      </c>
+    <row r="62" spans="7:7">
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="1" t="s">
-        <v>3919</v>
-      </c>
+    <row r="63" spans="7:7">
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="1" t="s">
-        <v>3920</v>
-      </c>
+    <row r="64" spans="7:7">
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="1" t="s">
-        <v>3921</v>
-      </c>
+    <row r="65" spans="7:7">
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="1" t="s">
-        <v>3922</v>
-      </c>
+    <row r="66" spans="7:7">
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="1" t="s">
-        <v>3923</v>
-      </c>
+    <row r="67" spans="7:7">
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="1" t="s">
-        <v>3924</v>
-      </c>
+    <row r="68" spans="7:7">
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="1" t="s">
-        <v>3925</v>
-      </c>
+    <row r="69" spans="7:7">
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7">
-      <c r="G70" s="1"/>
-    </row>
-    <row r="72" spans="1:7">
+    <row r="71" spans="7:7">
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="7:7">
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="7:7">
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="7:7">
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="7:7">
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="7:7">
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="7:7">
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="7:7">
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="7:7">
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="7:7">
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="7:7">
@@ -12700,14 +12583,11 @@
     <row r="108" spans="7:7">
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="7:7">
-      <c r="G109" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="C1:E250" xr:uid="{1B40E757-AF6D-418F-8CB6-C916F96CFF4A}"/>
+  <autoFilter ref="C1:E249" xr:uid="{1B40E757-AF6D-418F-8CB6-C916F96CFF4A}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A471:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
+  <conditionalFormatting sqref="A43:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="22"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="167" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -23230,10 +23110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C21679-A84C-4371-A1C5-AF880A10BEAA}">
-  <dimension ref="A1:V491"/>
+  <dimension ref="A1:X491"/>
   <sheetViews>
-    <sheetView topLeftCell="G35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V62" sqref="V62:V67"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23248,7 +23128,7 @@
     <col min="21" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -23312,8 +23192,14 @@
       <c r="V1" s="4">
         <v>44804</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" s="4">
+        <v>44805</v>
+      </c>
+      <c r="X1" s="4">
+        <v>44806</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -23377,8 +23263,14 @@
       <c r="V2" s="1" t="s">
         <v>3792</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2" s="1" t="s">
+        <v>3927</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="C3" s="1" t="s">
         <v>543</v>
       </c>
@@ -23439,8 +23331,14 @@
       <c r="V3" s="1" t="s">
         <v>3793</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3" s="1" t="s">
+        <v>3928</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>3976</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="C4" s="1" t="s">
         <v>544</v>
       </c>
@@ -23501,8 +23399,14 @@
       <c r="V4" s="1" t="s">
         <v>3794</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4" s="1" t="s">
+        <v>3929</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="C5" s="1" t="s">
         <v>545</v>
       </c>
@@ -23560,8 +23464,14 @@
       <c r="V5" s="1" t="s">
         <v>3795</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5" s="1" t="s">
+        <v>3930</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="C6" s="1" t="s">
         <v>546</v>
       </c>
@@ -23619,8 +23529,14 @@
       <c r="V6" s="1" t="s">
         <v>3796</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6" s="1" t="s">
+        <v>3931</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>3979</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="C7" s="1" t="s">
         <v>547</v>
       </c>
@@ -23678,8 +23594,14 @@
       <c r="V7" s="1" t="s">
         <v>3797</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7" s="1" t="s">
+        <v>3932</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="C8" s="1" t="s">
         <v>548</v>
       </c>
@@ -23737,8 +23659,14 @@
       <c r="V8" s="1" t="s">
         <v>3798</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8" s="1" t="s">
+        <v>3933</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>3981</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="C9" s="1" t="s">
         <v>549</v>
       </c>
@@ -23796,8 +23724,14 @@
       <c r="V9" s="1" t="s">
         <v>3799</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9" s="1" t="s">
+        <v>3934</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="C10" s="1" t="s">
         <v>550</v>
       </c>
@@ -23855,8 +23789,14 @@
       <c r="V10" s="1" t="s">
         <v>3800</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10" s="1" t="s">
+        <v>3935</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="C11" s="1" t="s">
         <v>551</v>
       </c>
@@ -23914,8 +23854,14 @@
       <c r="V11" s="1" t="s">
         <v>3801</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="W11" s="1" t="s">
+        <v>3936</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="C12" s="1" t="s">
         <v>552</v>
       </c>
@@ -23973,8 +23919,14 @@
       <c r="V12" s="1" t="s">
         <v>3802</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="W12" s="1" t="s">
+        <v>3937</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="C13" s="1" t="s">
         <v>553</v>
       </c>
@@ -24032,8 +23984,14 @@
       <c r="V13" s="1" t="s">
         <v>3803</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13" s="1" t="s">
+        <v>3938</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="C14" s="1" t="s">
         <v>554</v>
       </c>
@@ -24088,8 +24046,11 @@
       <c r="V14" s="1" t="s">
         <v>3804</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W14" s="1" t="s">
+        <v>3939</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="C15" s="1" t="s">
         <v>555</v>
       </c>
@@ -24144,8 +24105,11 @@
       <c r="V15" s="1" t="s">
         <v>3805</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="W15" s="1" t="s">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="C16" s="1" t="s">
         <v>556</v>
       </c>
@@ -24197,8 +24161,11 @@
       <c r="V16" s="1" t="s">
         <v>3806</v>
       </c>
-    </row>
-    <row r="17" spans="3:22">
+      <c r="W16" s="1" t="s">
+        <v>3941</v>
+      </c>
+    </row>
+    <row r="17" spans="3:23">
       <c r="C17" s="1" t="s">
         <v>557</v>
       </c>
@@ -24250,8 +24217,11 @@
       <c r="V17" s="1" t="s">
         <v>3807</v>
       </c>
-    </row>
-    <row r="18" spans="3:22">
+      <c r="W17" s="1" t="s">
+        <v>3942</v>
+      </c>
+    </row>
+    <row r="18" spans="3:23">
       <c r="C18" s="1" t="s">
         <v>558</v>
       </c>
@@ -24303,8 +24273,11 @@
       <c r="V18" s="1" t="s">
         <v>3808</v>
       </c>
-    </row>
-    <row r="19" spans="3:22">
+      <c r="W18" s="1" t="s">
+        <v>3943</v>
+      </c>
+    </row>
+    <row r="19" spans="3:23">
       <c r="C19" s="1" t="s">
         <v>559</v>
       </c>
@@ -24356,8 +24329,11 @@
       <c r="V19" s="1" t="s">
         <v>3809</v>
       </c>
-    </row>
-    <row r="20" spans="3:22">
+      <c r="W19" s="1" t="s">
+        <v>3944</v>
+      </c>
+    </row>
+    <row r="20" spans="3:23">
       <c r="C20" s="1" t="s">
         <v>560</v>
       </c>
@@ -24409,8 +24385,11 @@
       <c r="V20" s="1" t="s">
         <v>3810</v>
       </c>
-    </row>
-    <row r="21" spans="3:22">
+      <c r="W20" s="1" t="s">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="21" spans="3:23">
       <c r="C21" s="1" t="s">
         <v>561</v>
       </c>
@@ -24462,8 +24441,11 @@
       <c r="V21" s="1" t="s">
         <v>3811</v>
       </c>
-    </row>
-    <row r="22" spans="3:22">
+      <c r="W21" s="1" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="22" spans="3:23">
       <c r="C22" s="1" t="s">
         <v>562</v>
       </c>
@@ -24515,8 +24497,11 @@
       <c r="V22" s="1" t="s">
         <v>3812</v>
       </c>
-    </row>
-    <row r="23" spans="3:22">
+      <c r="W22" s="1" t="s">
+        <v>3947</v>
+      </c>
+    </row>
+    <row r="23" spans="3:23">
       <c r="C23" s="1" t="s">
         <v>563</v>
       </c>
@@ -24568,8 +24553,11 @@
       <c r="V23" s="1" t="s">
         <v>3813</v>
       </c>
-    </row>
-    <row r="24" spans="3:22">
+      <c r="W23" s="1" t="s">
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="24" spans="3:23">
       <c r="D24" s="1" t="s">
         <v>585</v>
       </c>
@@ -24618,8 +24606,11 @@
       <c r="V24" s="1" t="s">
         <v>3814</v>
       </c>
-    </row>
-    <row r="25" spans="3:22">
+      <c r="W24" s="1" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="25" spans="3:23">
       <c r="D25" s="1" t="s">
         <v>586</v>
       </c>
@@ -24668,8 +24659,11 @@
       <c r="V25" s="1" t="s">
         <v>3815</v>
       </c>
-    </row>
-    <row r="26" spans="3:22">
+      <c r="W25" s="1" t="s">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="26" spans="3:23">
       <c r="D26" s="1" t="s">
         <v>587</v>
       </c>
@@ -24718,8 +24712,11 @@
       <c r="V26" s="1" t="s">
         <v>3816</v>
       </c>
-    </row>
-    <row r="27" spans="3:22">
+      <c r="W26" s="1" t="s">
+        <v>3951</v>
+      </c>
+    </row>
+    <row r="27" spans="3:23">
       <c r="D27" s="1" t="s">
         <v>588</v>
       </c>
@@ -24768,8 +24765,11 @@
       <c r="V27" s="1" t="s">
         <v>3817</v>
       </c>
-    </row>
-    <row r="28" spans="3:22">
+      <c r="W27" s="1" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="28" spans="3:23">
       <c r="D28" s="1" t="s">
         <v>589</v>
       </c>
@@ -24818,8 +24818,11 @@
       <c r="V28" s="1" t="s">
         <v>3818</v>
       </c>
-    </row>
-    <row r="29" spans="3:22">
+      <c r="W28" s="1" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="29" spans="3:23">
       <c r="D29" s="1" t="s">
         <v>590</v>
       </c>
@@ -24868,8 +24871,11 @@
       <c r="V29" s="1" t="s">
         <v>3819</v>
       </c>
-    </row>
-    <row r="30" spans="3:22">
+      <c r="W29" s="1" t="s">
+        <v>3954</v>
+      </c>
+    </row>
+    <row r="30" spans="3:23">
       <c r="D30" s="1" t="s">
         <v>591</v>
       </c>
@@ -24918,8 +24924,11 @@
       <c r="V30" s="1" t="s">
         <v>3820</v>
       </c>
-    </row>
-    <row r="31" spans="3:22">
+      <c r="W30" s="1" t="s">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="31" spans="3:23">
       <c r="D31" s="1" t="s">
         <v>592</v>
       </c>
@@ -24968,8 +24977,11 @@
       <c r="V31" s="1" t="s">
         <v>3821</v>
       </c>
-    </row>
-    <row r="32" spans="3:22">
+      <c r="W31" s="1" t="s">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="32" spans="3:23">
       <c r="D32" s="1" t="s">
         <v>593</v>
       </c>
@@ -25018,8 +25030,11 @@
       <c r="V32" s="1" t="s">
         <v>3822</v>
       </c>
-    </row>
-    <row r="33" spans="4:22">
+      <c r="W32" s="1" t="s">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="33" spans="4:23">
       <c r="D33" s="1" t="s">
         <v>594</v>
       </c>
@@ -25068,8 +25083,11 @@
       <c r="V33" s="1" t="s">
         <v>3823</v>
       </c>
-    </row>
-    <row r="34" spans="4:22">
+      <c r="W33" s="1" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="34" spans="4:23">
       <c r="D34" s="1" t="s">
         <v>595</v>
       </c>
@@ -25118,8 +25136,11 @@
       <c r="V34" s="1" t="s">
         <v>3824</v>
       </c>
-    </row>
-    <row r="35" spans="4:22">
+      <c r="W34" s="1" t="s">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="35" spans="4:23">
       <c r="D35" s="1" t="s">
         <v>596</v>
       </c>
@@ -25168,8 +25189,11 @@
       <c r="V35" s="1" t="s">
         <v>3825</v>
       </c>
-    </row>
-    <row r="36" spans="4:22">
+      <c r="W35" s="1" t="s">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="36" spans="4:23">
       <c r="D36" s="1" t="s">
         <v>597</v>
       </c>
@@ -25218,8 +25242,11 @@
       <c r="V36" s="1" t="s">
         <v>3826</v>
       </c>
-    </row>
-    <row r="37" spans="4:22">
+      <c r="W36" s="1" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="37" spans="4:23">
       <c r="D37" s="1" t="s">
         <v>598</v>
       </c>
@@ -25268,8 +25295,11 @@
       <c r="V37" s="1" t="s">
         <v>3827</v>
       </c>
-    </row>
-    <row r="38" spans="4:22">
+      <c r="W37" s="1" t="s">
+        <v>3962</v>
+      </c>
+    </row>
+    <row r="38" spans="4:23">
       <c r="D38" s="1" t="s">
         <v>599</v>
       </c>
@@ -25318,8 +25348,11 @@
       <c r="V38" s="1" t="s">
         <v>3828</v>
       </c>
-    </row>
-    <row r="39" spans="4:22">
+      <c r="W38" s="1" t="s">
+        <v>3963</v>
+      </c>
+    </row>
+    <row r="39" spans="4:23">
       <c r="D39" s="1" t="s">
         <v>600</v>
       </c>
@@ -25368,8 +25401,11 @@
       <c r="V39" s="1" t="s">
         <v>3829</v>
       </c>
-    </row>
-    <row r="40" spans="4:22">
+      <c r="W39" s="1" t="s">
+        <v>3964</v>
+      </c>
+    </row>
+    <row r="40" spans="4:23">
       <c r="D40" s="1" t="s">
         <v>601</v>
       </c>
@@ -25418,8 +25454,11 @@
       <c r="V40" s="1" t="s">
         <v>3830</v>
       </c>
-    </row>
-    <row r="41" spans="4:22">
+      <c r="W40" s="1" t="s">
+        <v>3965</v>
+      </c>
+    </row>
+    <row r="41" spans="4:23">
       <c r="D41" s="1" t="s">
         <v>602</v>
       </c>
@@ -25468,8 +25507,11 @@
       <c r="V41" s="1" t="s">
         <v>3831</v>
       </c>
-    </row>
-    <row r="42" spans="4:22">
+      <c r="W41" s="1" t="s">
+        <v>3966</v>
+      </c>
+    </row>
+    <row r="42" spans="4:23">
       <c r="D42" s="1" t="s">
         <v>603</v>
       </c>
@@ -25518,8 +25560,11 @@
       <c r="V42" s="1" t="s">
         <v>3832</v>
       </c>
-    </row>
-    <row r="43" spans="4:22">
+      <c r="W42" s="1" t="s">
+        <v>3967</v>
+      </c>
+    </row>
+    <row r="43" spans="4:23">
       <c r="D43" s="1" t="s">
         <v>604</v>
       </c>
@@ -25568,8 +25613,11 @@
       <c r="V43" s="1" t="s">
         <v>3833</v>
       </c>
-    </row>
-    <row r="44" spans="4:22">
+      <c r="W43" s="1" t="s">
+        <v>3968</v>
+      </c>
+    </row>
+    <row r="44" spans="4:23">
       <c r="D44" s="1" t="s">
         <v>605</v>
       </c>
@@ -25618,8 +25666,11 @@
       <c r="V44" s="1" t="s">
         <v>3834</v>
       </c>
-    </row>
-    <row r="45" spans="4:22">
+      <c r="W44" s="1" t="s">
+        <v>3969</v>
+      </c>
+    </row>
+    <row r="45" spans="4:23">
       <c r="D45" s="1" t="s">
         <v>606</v>
       </c>
@@ -25668,8 +25719,11 @@
       <c r="V45" s="1" t="s">
         <v>3835</v>
       </c>
-    </row>
-    <row r="46" spans="4:22">
+      <c r="W45" s="1" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="46" spans="4:23">
       <c r="D46" s="1" t="s">
         <v>607</v>
       </c>
@@ -25718,8 +25772,11 @@
       <c r="V46" s="1" t="s">
         <v>3836</v>
       </c>
-    </row>
-    <row r="47" spans="4:22">
+      <c r="W46" s="1" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="47" spans="4:23">
       <c r="D47" s="1" t="s">
         <v>608</v>
       </c>
@@ -25768,8 +25825,11 @@
       <c r="V47" s="1" t="s">
         <v>3837</v>
       </c>
-    </row>
-    <row r="48" spans="4:22">
+      <c r="W47" s="1" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="48" spans="4:23">
       <c r="D48" s="1" t="s">
         <v>609</v>
       </c>
@@ -25815,8 +25875,11 @@
       <c r="V48" s="1" t="s">
         <v>3838</v>
       </c>
-    </row>
-    <row r="49" spans="4:22">
+      <c r="W48" s="1" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="49" spans="4:23">
       <c r="D49" s="1" t="s">
         <v>610</v>
       </c>
@@ -25862,8 +25925,11 @@
       <c r="V49" s="1" t="s">
         <v>3839</v>
       </c>
-    </row>
-    <row r="50" spans="4:22">
+      <c r="W49" s="1" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="50" spans="4:23">
       <c r="D50" s="1" t="s">
         <v>611</v>
       </c>
@@ -25910,7 +25976,7 @@
         <v>3840</v>
       </c>
     </row>
-    <row r="51" spans="4:22">
+    <row r="51" spans="4:23">
       <c r="D51" s="1" t="s">
         <v>612</v>
       </c>
@@ -25957,7 +26023,7 @@
         <v>3841</v>
       </c>
     </row>
-    <row r="52" spans="4:22">
+    <row r="52" spans="4:23">
       <c r="D52" s="1" t="s">
         <v>613</v>
       </c>
@@ -26004,7 +26070,7 @@
         <v>3842</v>
       </c>
     </row>
-    <row r="53" spans="4:22">
+    <row r="53" spans="4:23">
       <c r="D53" s="1" t="s">
         <v>614</v>
       </c>
@@ -26051,7 +26117,7 @@
         <v>3843</v>
       </c>
     </row>
-    <row r="54" spans="4:22">
+    <row r="54" spans="4:23">
       <c r="D54" s="1" t="s">
         <v>615</v>
       </c>
@@ -26098,7 +26164,7 @@
         <v>3844</v>
       </c>
     </row>
-    <row r="55" spans="4:22">
+    <row r="55" spans="4:23">
       <c r="D55" s="1" t="s">
         <v>616</v>
       </c>
@@ -26145,7 +26211,7 @@
         <v>3845</v>
       </c>
     </row>
-    <row r="56" spans="4:22">
+    <row r="56" spans="4:23">
       <c r="D56" s="1" t="s">
         <v>617</v>
       </c>
@@ -26192,7 +26258,7 @@
         <v>3846</v>
       </c>
     </row>
-    <row r="57" spans="4:22">
+    <row r="57" spans="4:23">
       <c r="D57" s="1" t="s">
         <v>618</v>
       </c>
@@ -26239,7 +26305,7 @@
         <v>3847</v>
       </c>
     </row>
-    <row r="58" spans="4:22">
+    <row r="58" spans="4:23">
       <c r="D58" s="1" t="s">
         <v>619</v>
       </c>
@@ -26286,7 +26352,7 @@
         <v>3848</v>
       </c>
     </row>
-    <row r="59" spans="4:22">
+    <row r="59" spans="4:23">
       <c r="D59" s="1" t="s">
         <v>620</v>
       </c>
@@ -26330,7 +26396,7 @@
         <v>3849</v>
       </c>
     </row>
-    <row r="60" spans="4:22">
+    <row r="60" spans="4:23">
       <c r="D60" s="1" t="s">
         <v>621</v>
       </c>
@@ -26374,7 +26440,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="61" spans="4:22">
+    <row r="61" spans="4:23">
       <c r="D61" s="1" t="s">
         <v>622</v>
       </c>
@@ -26418,7 +26484,7 @@
         <v>3851</v>
       </c>
     </row>
-    <row r="62" spans="4:22">
+    <row r="62" spans="4:23">
       <c r="D62" s="1" t="s">
         <v>623</v>
       </c>
@@ -26462,7 +26528,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="63" spans="4:22">
+    <row r="63" spans="4:23">
       <c r="D63" s="1" t="s">
         <v>624</v>
       </c>
@@ -26506,7 +26572,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="64" spans="4:22">
+    <row r="64" spans="4:23">
       <c r="D64" s="1" t="s">
         <v>625</v>
       </c>
@@ -26722,6 +26788,9 @@
       <c r="U68" s="1" t="s">
         <v>3705</v>
       </c>
+      <c r="V68" s="1" t="s">
+        <v>3857</v>
+      </c>
     </row>
     <row r="69" spans="4:22">
       <c r="D69" s="1" t="s">
@@ -26763,6 +26832,9 @@
       <c r="U69" s="1" t="s">
         <v>3706</v>
       </c>
+      <c r="V69" s="1" t="s">
+        <v>3858</v>
+      </c>
     </row>
     <row r="70" spans="4:22">
       <c r="D70" s="1" t="s">
@@ -26804,6 +26876,9 @@
       <c r="U70" s="1" t="s">
         <v>3707</v>
       </c>
+      <c r="V70" s="1" t="s">
+        <v>3859</v>
+      </c>
     </row>
     <row r="71" spans="4:22">
       <c r="D71" s="1" t="s">
@@ -26842,6 +26917,9 @@
       <c r="U71" s="1" t="s">
         <v>3708</v>
       </c>
+      <c r="V71" s="1" t="s">
+        <v>3860</v>
+      </c>
     </row>
     <row r="72" spans="4:22">
       <c r="E72" s="5" t="s">
@@ -26877,6 +26955,9 @@
       <c r="U72" s="1" t="s">
         <v>3709</v>
       </c>
+      <c r="V72" s="1" t="s">
+        <v>3861</v>
+      </c>
     </row>
     <row r="73" spans="4:22">
       <c r="E73" s="5" t="s">
@@ -26915,6 +26996,9 @@
       <c r="U73" s="1" t="s">
         <v>3710</v>
       </c>
+      <c r="V73" s="1" t="s">
+        <v>3862</v>
+      </c>
     </row>
     <row r="74" spans="4:22">
       <c r="E74" s="5" t="s">
@@ -26953,6 +27037,9 @@
       <c r="U74" s="1" t="s">
         <v>3711</v>
       </c>
+      <c r="V74" s="1" t="s">
+        <v>3863</v>
+      </c>
     </row>
     <row r="75" spans="4:22">
       <c r="E75" s="5" t="s">
@@ -26991,6 +27078,9 @@
       <c r="U75" s="1" t="s">
         <v>3712</v>
       </c>
+      <c r="V75" s="1" t="s">
+        <v>3864</v>
+      </c>
     </row>
     <row r="76" spans="4:22">
       <c r="E76" s="5" t="s">
@@ -27029,6 +27119,9 @@
       <c r="U76" s="1" t="s">
         <v>3713</v>
       </c>
+      <c r="V76" s="1" t="s">
+        <v>3865</v>
+      </c>
     </row>
     <row r="77" spans="4:22">
       <c r="E77" s="5" t="s">
@@ -27067,6 +27160,9 @@
       <c r="U77" s="1" t="s">
         <v>3714</v>
       </c>
+      <c r="V77" s="1" t="s">
+        <v>3866</v>
+      </c>
     </row>
     <row r="78" spans="4:22">
       <c r="E78" s="5" t="s">
@@ -27105,6 +27201,9 @@
       <c r="U78" s="1" t="s">
         <v>3715</v>
       </c>
+      <c r="V78" s="1" t="s">
+        <v>3867</v>
+      </c>
     </row>
     <row r="79" spans="4:22">
       <c r="E79" s="5" t="s">
@@ -27143,6 +27242,9 @@
       <c r="U79" s="1" t="s">
         <v>3716</v>
       </c>
+      <c r="V79" s="1" t="s">
+        <v>3868</v>
+      </c>
     </row>
     <row r="80" spans="4:22">
       <c r="E80" s="5" t="s">
@@ -27181,8 +27283,11 @@
       <c r="U80" s="1" t="s">
         <v>3717</v>
       </c>
-    </row>
-    <row r="81" spans="5:21">
+      <c r="V80" s="1" t="s">
+        <v>3869</v>
+      </c>
+    </row>
+    <row r="81" spans="5:22">
       <c r="E81" s="1" t="s">
         <v>712</v>
       </c>
@@ -27219,8 +27324,11 @@
       <c r="U81" s="1" t="s">
         <v>3718</v>
       </c>
-    </row>
-    <row r="82" spans="5:21">
+      <c r="V81" s="1" t="s">
+        <v>3870</v>
+      </c>
+    </row>
+    <row r="82" spans="5:22">
       <c r="E82" s="1" t="s">
         <v>713</v>
       </c>
@@ -27257,8 +27365,11 @@
       <c r="U82" s="1" t="s">
         <v>3719</v>
       </c>
-    </row>
-    <row r="83" spans="5:21">
+      <c r="V82" s="1" t="s">
+        <v>3871</v>
+      </c>
+    </row>
+    <row r="83" spans="5:22">
       <c r="E83" s="1" t="s">
         <v>714</v>
       </c>
@@ -27295,8 +27406,11 @@
       <c r="U83" s="1" t="s">
         <v>3720</v>
       </c>
-    </row>
-    <row r="84" spans="5:21">
+      <c r="V83" s="1" t="s">
+        <v>3872</v>
+      </c>
+    </row>
+    <row r="84" spans="5:22">
       <c r="E84" s="1" t="s">
         <v>715</v>
       </c>
@@ -27333,8 +27447,11 @@
       <c r="U84" s="1" t="s">
         <v>3721</v>
       </c>
-    </row>
-    <row r="85" spans="5:21">
+      <c r="V84" s="1" t="s">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="85" spans="5:22">
       <c r="E85" s="1" t="s">
         <v>716</v>
       </c>
@@ -27371,8 +27488,11 @@
       <c r="U85" s="1" t="s">
         <v>3722</v>
       </c>
-    </row>
-    <row r="86" spans="5:21">
+      <c r="V85" s="1" t="s">
+        <v>3874</v>
+      </c>
+    </row>
+    <row r="86" spans="5:22">
       <c r="E86" s="1" t="s">
         <v>717</v>
       </c>
@@ -27409,8 +27529,11 @@
       <c r="U86" s="1" t="s">
         <v>3723</v>
       </c>
-    </row>
-    <row r="87" spans="5:21">
+      <c r="V86" s="1" t="s">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="87" spans="5:22">
       <c r="E87" s="1" t="s">
         <v>718</v>
       </c>
@@ -27447,8 +27570,11 @@
       <c r="U87" s="1" t="s">
         <v>3724</v>
       </c>
-    </row>
-    <row r="88" spans="5:21">
+      <c r="V87" s="1" t="s">
+        <v>3876</v>
+      </c>
+    </row>
+    <row r="88" spans="5:22">
       <c r="E88" s="1" t="s">
         <v>719</v>
       </c>
@@ -27485,8 +27611,11 @@
       <c r="U88" s="1" t="s">
         <v>3725</v>
       </c>
-    </row>
-    <row r="89" spans="5:21">
+      <c r="V88" s="1" t="s">
+        <v>3877</v>
+      </c>
+    </row>
+    <row r="89" spans="5:22">
       <c r="E89" s="1" t="s">
         <v>720</v>
       </c>
@@ -27520,8 +27649,11 @@
       <c r="U89" s="1" t="s">
         <v>3726</v>
       </c>
-    </row>
-    <row r="90" spans="5:21">
+      <c r="V89" s="1" t="s">
+        <v>3878</v>
+      </c>
+    </row>
+    <row r="90" spans="5:22">
       <c r="E90" s="1" t="s">
         <v>721</v>
       </c>
@@ -27555,8 +27687,11 @@
       <c r="U90" s="1" t="s">
         <v>3727</v>
       </c>
-    </row>
-    <row r="91" spans="5:21">
+      <c r="V90" s="1" t="s">
+        <v>3879</v>
+      </c>
+    </row>
+    <row r="91" spans="5:22">
       <c r="E91" s="1" t="s">
         <v>722</v>
       </c>
@@ -27590,8 +27725,11 @@
       <c r="U91" s="1" t="s">
         <v>3728</v>
       </c>
-    </row>
-    <row r="92" spans="5:21">
+      <c r="V91" s="1" t="s">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="92" spans="5:22">
       <c r="E92" s="1" t="s">
         <v>723</v>
       </c>
@@ -27625,8 +27763,11 @@
       <c r="U92" s="1" t="s">
         <v>3729</v>
       </c>
-    </row>
-    <row r="93" spans="5:21">
+      <c r="V92" s="1" t="s">
+        <v>3881</v>
+      </c>
+    </row>
+    <row r="93" spans="5:22">
       <c r="E93" s="1" t="s">
         <v>724</v>
       </c>
@@ -27660,8 +27801,11 @@
       <c r="U93" s="1" t="s">
         <v>3730</v>
       </c>
-    </row>
-    <row r="94" spans="5:21">
+      <c r="V93" s="1" t="s">
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="94" spans="5:22">
       <c r="E94" s="1" t="s">
         <v>725</v>
       </c>
@@ -27695,8 +27839,11 @@
       <c r="U94" s="1" t="s">
         <v>3731</v>
       </c>
-    </row>
-    <row r="95" spans="5:21">
+      <c r="V94" s="1" t="s">
+        <v>3883</v>
+      </c>
+    </row>
+    <row r="95" spans="5:22">
       <c r="E95" s="1" t="s">
         <v>726</v>
       </c>
@@ -27730,8 +27877,11 @@
       <c r="U95" s="1" t="s">
         <v>3732</v>
       </c>
-    </row>
-    <row r="96" spans="5:21">
+      <c r="V95" s="1" t="s">
+        <v>3884</v>
+      </c>
+    </row>
+    <row r="96" spans="5:22">
       <c r="E96" s="1" t="s">
         <v>727</v>
       </c>
@@ -27765,8 +27915,11 @@
       <c r="U96" s="1" t="s">
         <v>3733</v>
       </c>
-    </row>
-    <row r="97" spans="5:21">
+      <c r="V96" s="1" t="s">
+        <v>3885</v>
+      </c>
+    </row>
+    <row r="97" spans="5:22">
       <c r="E97" s="1" t="s">
         <v>728</v>
       </c>
@@ -27800,8 +27953,11 @@
       <c r="U97" s="1" t="s">
         <v>3734</v>
       </c>
-    </row>
-    <row r="98" spans="5:21">
+      <c r="V97" s="1" t="s">
+        <v>3886</v>
+      </c>
+    </row>
+    <row r="98" spans="5:22">
       <c r="E98" s="1" t="s">
         <v>729</v>
       </c>
@@ -27835,8 +27991,11 @@
       <c r="U98" s="1" t="s">
         <v>3735</v>
       </c>
-    </row>
-    <row r="99" spans="5:21">
+      <c r="V98" s="1" t="s">
+        <v>3887</v>
+      </c>
+    </row>
+    <row r="99" spans="5:22">
       <c r="E99" s="1" t="s">
         <v>730</v>
       </c>
@@ -27870,8 +28029,11 @@
       <c r="U99" s="1" t="s">
         <v>3736</v>
       </c>
-    </row>
-    <row r="100" spans="5:21">
+      <c r="V99" s="1" t="s">
+        <v>3888</v>
+      </c>
+    </row>
+    <row r="100" spans="5:22">
       <c r="E100" s="1" t="s">
         <v>731</v>
       </c>
@@ -27905,8 +28067,11 @@
       <c r="U100" s="1" t="s">
         <v>3737</v>
       </c>
-    </row>
-    <row r="101" spans="5:21">
+      <c r="V100" s="1" t="s">
+        <v>3889</v>
+      </c>
+    </row>
+    <row r="101" spans="5:22">
       <c r="E101" s="1" t="s">
         <v>732</v>
       </c>
@@ -27940,8 +28105,11 @@
       <c r="U101" s="1" t="s">
         <v>3738</v>
       </c>
-    </row>
-    <row r="102" spans="5:21">
+      <c r="V101" s="1" t="s">
+        <v>3890</v>
+      </c>
+    </row>
+    <row r="102" spans="5:22">
       <c r="E102" s="1" t="s">
         <v>733</v>
       </c>
@@ -27975,8 +28143,11 @@
       <c r="U102" s="1" t="s">
         <v>3739</v>
       </c>
-    </row>
-    <row r="103" spans="5:21">
+      <c r="V102" s="1" t="s">
+        <v>3891</v>
+      </c>
+    </row>
+    <row r="103" spans="5:22">
       <c r="E103" s="1" t="s">
         <v>734</v>
       </c>
@@ -28010,8 +28181,11 @@
       <c r="U103" s="1" t="s">
         <v>3740</v>
       </c>
-    </row>
-    <row r="104" spans="5:21">
+      <c r="V103" s="1" t="s">
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="104" spans="5:22">
       <c r="E104" s="1" t="s">
         <v>735</v>
       </c>
@@ -28045,8 +28219,11 @@
       <c r="U104" s="1" t="s">
         <v>3741</v>
       </c>
-    </row>
-    <row r="105" spans="5:21">
+      <c r="V104" s="1" t="s">
+        <v>3893</v>
+      </c>
+    </row>
+    <row r="105" spans="5:22">
       <c r="E105" s="1" t="s">
         <v>736</v>
       </c>
@@ -28080,8 +28257,11 @@
       <c r="U105" s="1" t="s">
         <v>3742</v>
       </c>
-    </row>
-    <row r="106" spans="5:21">
+      <c r="V105" s="1" t="s">
+        <v>3894</v>
+      </c>
+    </row>
+    <row r="106" spans="5:22">
       <c r="E106" s="1" t="s">
         <v>737</v>
       </c>
@@ -28115,8 +28295,11 @@
       <c r="U106" s="1" t="s">
         <v>3743</v>
       </c>
-    </row>
-    <row r="107" spans="5:21">
+      <c r="V106" s="1" t="s">
+        <v>3895</v>
+      </c>
+    </row>
+    <row r="107" spans="5:22">
       <c r="E107" s="1" t="s">
         <v>738</v>
       </c>
@@ -28150,8 +28333,11 @@
       <c r="U107" s="1" t="s">
         <v>3744</v>
       </c>
-    </row>
-    <row r="108" spans="5:21">
+      <c r="V107" s="1" t="s">
+        <v>3896</v>
+      </c>
+    </row>
+    <row r="108" spans="5:22">
       <c r="E108" s="1" t="s">
         <v>739</v>
       </c>
@@ -28185,8 +28371,11 @@
       <c r="U108" s="1" t="s">
         <v>3745</v>
       </c>
-    </row>
-    <row r="109" spans="5:21">
+      <c r="V108" s="1" t="s">
+        <v>3897</v>
+      </c>
+    </row>
+    <row r="109" spans="5:22">
       <c r="E109" s="1" t="s">
         <v>740</v>
       </c>
@@ -28220,8 +28409,11 @@
       <c r="U109" s="1" t="s">
         <v>3746</v>
       </c>
-    </row>
-    <row r="110" spans="5:21">
+      <c r="V109" s="1" t="s">
+        <v>3898</v>
+      </c>
+    </row>
+    <row r="110" spans="5:22">
       <c r="E110" s="1" t="s">
         <v>741</v>
       </c>
@@ -28255,8 +28447,11 @@
       <c r="U110" s="1" t="s">
         <v>3747</v>
       </c>
-    </row>
-    <row r="111" spans="5:21">
+      <c r="V110" s="1" t="s">
+        <v>3899</v>
+      </c>
+    </row>
+    <row r="111" spans="5:22">
       <c r="E111" s="1" t="s">
         <v>742</v>
       </c>
@@ -28290,8 +28485,11 @@
       <c r="U111" s="1" t="s">
         <v>3748</v>
       </c>
-    </row>
-    <row r="112" spans="5:21">
+      <c r="V111" s="1" t="s">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="112" spans="5:22">
       <c r="E112" s="1" t="s">
         <v>743</v>
       </c>
@@ -28325,8 +28523,11 @@
       <c r="U112" s="1" t="s">
         <v>3749</v>
       </c>
-    </row>
-    <row r="113" spans="5:21">
+      <c r="V112" s="1" t="s">
+        <v>3901</v>
+      </c>
+    </row>
+    <row r="113" spans="5:22">
       <c r="E113" s="1" t="s">
         <v>744</v>
       </c>
@@ -28360,8 +28561,11 @@
       <c r="U113" s="1" t="s">
         <v>3750</v>
       </c>
-    </row>
-    <row r="114" spans="5:21">
+      <c r="V113" s="1" t="s">
+        <v>3902</v>
+      </c>
+    </row>
+    <row r="114" spans="5:22">
       <c r="E114" s="1" t="s">
         <v>745</v>
       </c>
@@ -28392,8 +28596,11 @@
       <c r="U114" s="1" t="s">
         <v>3751</v>
       </c>
-    </row>
-    <row r="115" spans="5:21">
+      <c r="V114" s="1" t="s">
+        <v>3903</v>
+      </c>
+    </row>
+    <row r="115" spans="5:22">
       <c r="E115" s="1" t="s">
         <v>746</v>
       </c>
@@ -28424,8 +28631,11 @@
       <c r="U115" s="1" t="s">
         <v>3752</v>
       </c>
-    </row>
-    <row r="116" spans="5:21">
+      <c r="V115" s="1" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="116" spans="5:22">
       <c r="E116" s="1" t="s">
         <v>747</v>
       </c>
@@ -28456,8 +28666,11 @@
       <c r="U116" s="1" t="s">
         <v>3753</v>
       </c>
-    </row>
-    <row r="117" spans="5:21">
+      <c r="V116" s="1" t="s">
+        <v>3905</v>
+      </c>
+    </row>
+    <row r="117" spans="5:22">
       <c r="E117" s="1" t="s">
         <v>748</v>
       </c>
@@ -28488,8 +28701,11 @@
       <c r="U117" s="1" t="s">
         <v>3754</v>
       </c>
-    </row>
-    <row r="118" spans="5:21">
+      <c r="V117" s="1" t="s">
+        <v>3906</v>
+      </c>
+    </row>
+    <row r="118" spans="5:22">
       <c r="E118" s="1" t="s">
         <v>749</v>
       </c>
@@ -28520,8 +28736,11 @@
       <c r="U118" s="1" t="s">
         <v>3755</v>
       </c>
-    </row>
-    <row r="119" spans="5:21">
+      <c r="V118" s="1" t="s">
+        <v>3907</v>
+      </c>
+    </row>
+    <row r="119" spans="5:22">
       <c r="E119" s="1" t="s">
         <v>750</v>
       </c>
@@ -28552,8 +28771,11 @@
       <c r="U119" s="1" t="s">
         <v>3756</v>
       </c>
-    </row>
-    <row r="120" spans="5:21">
+      <c r="V119" s="1" t="s">
+        <v>3908</v>
+      </c>
+    </row>
+    <row r="120" spans="5:22">
       <c r="E120" s="1" t="s">
         <v>751</v>
       </c>
@@ -28584,8 +28806,11 @@
       <c r="U120" s="1" t="s">
         <v>3757</v>
       </c>
-    </row>
-    <row r="121" spans="5:21">
+      <c r="V120" s="1" t="s">
+        <v>3909</v>
+      </c>
+    </row>
+    <row r="121" spans="5:22">
       <c r="E121" s="1" t="s">
         <v>752</v>
       </c>
@@ -28616,8 +28841,11 @@
       <c r="U121" s="1" t="s">
         <v>3758</v>
       </c>
-    </row>
-    <row r="122" spans="5:21">
+      <c r="V121" s="1" t="s">
+        <v>3910</v>
+      </c>
+    </row>
+    <row r="122" spans="5:22">
       <c r="E122" s="1" t="s">
         <v>753</v>
       </c>
@@ -28648,8 +28876,11 @@
       <c r="U122" s="1" t="s">
         <v>3759</v>
       </c>
-    </row>
-    <row r="123" spans="5:21">
+      <c r="V122" s="1" t="s">
+        <v>3911</v>
+      </c>
+    </row>
+    <row r="123" spans="5:22">
       <c r="E123" s="1" t="s">
         <v>754</v>
       </c>
@@ -28680,8 +28911,11 @@
       <c r="U123" s="1" t="s">
         <v>3760</v>
       </c>
-    </row>
-    <row r="124" spans="5:21">
+      <c r="V123" s="1" t="s">
+        <v>3912</v>
+      </c>
+    </row>
+    <row r="124" spans="5:22">
       <c r="E124" s="1" t="s">
         <v>755</v>
       </c>
@@ -28712,8 +28946,11 @@
       <c r="U124" s="1" t="s">
         <v>3761</v>
       </c>
-    </row>
-    <row r="125" spans="5:21">
+      <c r="V124" s="1" t="s">
+        <v>3913</v>
+      </c>
+    </row>
+    <row r="125" spans="5:22">
       <c r="E125" s="1" t="s">
         <v>756</v>
       </c>
@@ -28744,8 +28981,11 @@
       <c r="U125" s="1" t="s">
         <v>3762</v>
       </c>
-    </row>
-    <row r="126" spans="5:21">
+      <c r="V125" s="1" t="s">
+        <v>3914</v>
+      </c>
+    </row>
+    <row r="126" spans="5:22">
       <c r="E126" s="1" t="s">
         <v>757</v>
       </c>
@@ -28776,8 +29016,11 @@
       <c r="U126" s="1" t="s">
         <v>3763</v>
       </c>
-    </row>
-    <row r="127" spans="5:21">
+      <c r="V126" s="1" t="s">
+        <v>3915</v>
+      </c>
+    </row>
+    <row r="127" spans="5:22">
       <c r="E127" s="1" t="s">
         <v>758</v>
       </c>
@@ -28808,8 +29051,11 @@
       <c r="U127" s="1" t="s">
         <v>3764</v>
       </c>
-    </row>
-    <row r="128" spans="5:21">
+      <c r="V127" s="1" t="s">
+        <v>3916</v>
+      </c>
+    </row>
+    <row r="128" spans="5:22">
       <c r="E128" s="1" t="s">
         <v>759</v>
       </c>
@@ -28840,8 +29086,11 @@
       <c r="U128" s="1" t="s">
         <v>3765</v>
       </c>
-    </row>
-    <row r="129" spans="5:21">
+      <c r="V128" s="1" t="s">
+        <v>3917</v>
+      </c>
+    </row>
+    <row r="129" spans="5:22">
       <c r="E129" s="1" t="s">
         <v>760</v>
       </c>
@@ -28872,8 +29121,11 @@
       <c r="U129" s="1" t="s">
         <v>3766</v>
       </c>
-    </row>
-    <row r="130" spans="5:21">
+      <c r="V129" s="1" t="s">
+        <v>3918</v>
+      </c>
+    </row>
+    <row r="130" spans="5:22">
       <c r="E130" s="1" t="s">
         <v>761</v>
       </c>
@@ -28904,8 +29156,11 @@
       <c r="U130" s="1" t="s">
         <v>3767</v>
       </c>
-    </row>
-    <row r="131" spans="5:21">
+      <c r="V130" s="1" t="s">
+        <v>3919</v>
+      </c>
+    </row>
+    <row r="131" spans="5:22">
       <c r="E131" s="1" t="s">
         <v>762</v>
       </c>
@@ -28936,8 +29191,11 @@
       <c r="U131" s="1" t="s">
         <v>3768</v>
       </c>
-    </row>
-    <row r="132" spans="5:21">
+      <c r="V131" s="1" t="s">
+        <v>3920</v>
+      </c>
+    </row>
+    <row r="132" spans="5:22">
       <c r="E132" s="1" t="s">
         <v>763</v>
       </c>
@@ -28968,8 +29226,11 @@
       <c r="U132" s="1" t="s">
         <v>3769</v>
       </c>
-    </row>
-    <row r="133" spans="5:21">
+      <c r="V132" s="1" t="s">
+        <v>3921</v>
+      </c>
+    </row>
+    <row r="133" spans="5:22">
       <c r="E133" s="1" t="s">
         <v>764</v>
       </c>
@@ -29000,8 +29261,11 @@
       <c r="U133" s="1" t="s">
         <v>3770</v>
       </c>
-    </row>
-    <row r="134" spans="5:21">
+      <c r="V133" s="1" t="s">
+        <v>3922</v>
+      </c>
+    </row>
+    <row r="134" spans="5:22">
       <c r="E134" s="1" t="s">
         <v>765</v>
       </c>
@@ -29032,8 +29296,11 @@
       <c r="U134" s="1" t="s">
         <v>3771</v>
       </c>
-    </row>
-    <row r="135" spans="5:21">
+      <c r="V134" s="1" t="s">
+        <v>3923</v>
+      </c>
+    </row>
+    <row r="135" spans="5:22">
       <c r="E135" s="1" t="s">
         <v>766</v>
       </c>
@@ -29064,8 +29331,11 @@
       <c r="U135" s="1" t="s">
         <v>3772</v>
       </c>
-    </row>
-    <row r="136" spans="5:21">
+      <c r="V135" s="1" t="s">
+        <v>3924</v>
+      </c>
+    </row>
+    <row r="136" spans="5:22">
       <c r="E136" s="1" t="s">
         <v>767</v>
       </c>
@@ -29096,8 +29366,11 @@
       <c r="U136" s="1" t="s">
         <v>3773</v>
       </c>
-    </row>
-    <row r="137" spans="5:21">
+      <c r="V136" s="1" t="s">
+        <v>3925</v>
+      </c>
+    </row>
+    <row r="137" spans="5:22">
       <c r="E137" s="1" t="s">
         <v>768</v>
       </c>
@@ -29129,7 +29402,7 @@
         <v>3774</v>
       </c>
     </row>
-    <row r="138" spans="5:21">
+    <row r="138" spans="5:22">
       <c r="E138" s="1" t="s">
         <v>769</v>
       </c>
@@ -29161,7 +29434,7 @@
         <v>3775</v>
       </c>
     </row>
-    <row r="139" spans="5:21">
+    <row r="139" spans="5:22">
       <c r="E139" s="1" t="s">
         <v>770</v>
       </c>
@@ -29193,7 +29466,7 @@
         <v>3776</v>
       </c>
     </row>
-    <row r="140" spans="5:21">
+    <row r="140" spans="5:22">
       <c r="E140" s="1" t="s">
         <v>771</v>
       </c>
@@ -29225,7 +29498,7 @@
         <v>3777</v>
       </c>
     </row>
-    <row r="141" spans="5:21">
+    <row r="141" spans="5:22">
       <c r="E141" s="1" t="s">
         <v>772</v>
       </c>
@@ -29257,7 +29530,7 @@
         <v>3778</v>
       </c>
     </row>
-    <row r="142" spans="5:21">
+    <row r="142" spans="5:22">
       <c r="E142" s="1" t="s">
         <v>773</v>
       </c>
@@ -29289,7 +29562,7 @@
         <v>3779</v>
       </c>
     </row>
-    <row r="143" spans="5:21">
+    <row r="143" spans="5:22">
       <c r="E143" s="1" t="s">
         <v>774</v>
       </c>
@@ -29321,7 +29594,7 @@
         <v>3780</v>
       </c>
     </row>
-    <row r="144" spans="5:21">
+    <row r="144" spans="5:22">
       <c r="E144" s="1" t="s">
         <v>775</v>
       </c>
@@ -34320,6 +34593,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="W8:W49">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>